<commit_message>
facturas excell y pdf
</commit_message>
<xml_diff>
--- a/ProyectoERP/wwwroot/facturas/FACTURA.XLSX
+++ b/ProyectoERP/wwwroot/facturas/FACTURA.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sara Álvarez\Desktop\FULLSTACK\NETCORE\ProyectoERP\ProyectoERP\wwwroot\facturas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112BC31D-A808-441D-87D7-29AD68D0B941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB102F0F-72D6-4C73-A264-75208232F2A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,18 +37,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
-    <t>B87886792</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C/ LIBERTAD, 37 1ª PLANTA </t>
-  </si>
-  <si>
-    <t>OFICINA 2A6 - C.P. 28936</t>
-  </si>
-  <si>
-    <t>MÓSTOLES (MADRID)</t>
-  </si>
-  <si>
     <t>FACTURA</t>
   </si>
   <si>
@@ -79,7 +67,19 @@
     <t>POBLACIÓN: MADRID</t>
   </si>
   <si>
-    <t>EXEM, S.L.</t>
+    <t>B12121212</t>
+  </si>
+  <si>
+    <t>EJEMPLO, S.L.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C/EJEMPLO, 2 1ª PLANTA </t>
+  </si>
+  <si>
+    <t>OFICINA 1B9 - C.P. 28800</t>
+  </si>
+  <si>
+    <t>EJEMPLO (MADRID)</t>
   </si>
 </sst>
 </file>
@@ -275,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -296,6 +296,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -329,17 +332,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -680,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A6:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:D11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -694,82 +692,80 @@
   <sheetData>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6" s="16"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="13" spans="1:7" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C13" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="19"/>
+      <c r="C13" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="20"/>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G16" s="2">
         <v>1</v>
       </c>
+      <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E17" s="4"/>
       <c r="F17" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="22"/>
+        <v>3</v>
+      </c>
+      <c r="B18" s="21"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="23"/>
       <c r="F18" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G18" s="17"/>
     </row>
     <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="26"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" s="24"/>
-      <c r="G19" s="25"/>
+        <v>4</v>
+      </c>
+      <c r="B19" s="27"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="25"/>
+      <c r="G19" s="26"/>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="32"/>
-      <c r="B21" s="33"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
@@ -778,27 +774,25 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="30" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B22" s="31"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="G22" s="13">
-        <v>20.66</v>
-      </c>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="8"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
       <c r="G23" s="9"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
       <c r="G24" s="9"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -808,11 +802,11 @@
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
       <c r="D26" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G26" s="13">
         <f>G22*0.21</f>
-        <v>4.3385999999999996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -831,7 +825,7 @@
     <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -840,7 +834,7 @@
       <c r="F30" s="7"/>
       <c r="G30" s="15">
         <f>G22+G26</f>
-        <v>24.9986</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>